<commit_message>
Oublie du tableau de synthèse
</commit_message>
<xml_diff>
--- a/assets/img/Tableau de synthèse - Epreuve E4 - BTS SIO 2023 - ROUSSEL Paul.xlsb.xlsx
+++ b/assets/img/Tableau de synthèse - Epreuve E4 - BTS SIO 2023 - ROUSSEL Paul.xlsb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\firep\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88FFE37A-10F5-419C-94D0-C1D099D79C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F531BB2-ADE8-47E5-9BA7-73F7889CB443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$35</definedName>
   </definedNames>
   <calcPr calcId="101716"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -108,9 +107,6 @@
     <t>Réalisations en milieu professionnel en cours de seconde année</t>
   </si>
   <si>
-    <t>Adresse URL du portfolio :</t>
-  </si>
-  <si>
     <t>NOM et prénom : ROUSSEL Paul</t>
   </si>
   <si>
@@ -157,6 +153,9 @@
   </si>
   <si>
     <t>08/01/2024 - 09/02/2024</t>
+  </si>
+  <si>
+    <t>Adresse URL du portfolio : https://paulairenp.github.io/Portfolio/</t>
   </si>
 </sst>
 </file>
@@ -711,9 +710,48 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -736,45 +774,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1087,8 +1086,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1101,56 +1100,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="28"/>
+    </row>
+    <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+    </row>
+    <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="26"/>
-    </row>
-    <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-    </row>
-    <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="34"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="47"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="32"/>
+      <c r="A4" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="45"/>
       <c r="F4" s="14" t="s">
         <v>8</v>
       </c>
@@ -1158,26 +1157,26 @@
         <v>15</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="47"/>
+      <c r="A5" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="39"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="35" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1200,8 +1199,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
-      <c r="B7" s="44"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="23" t="s">
         <v>9</v>
       </c>
@@ -1257,16 +1256,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="39"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1305,13 +1304,13 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="24">
         <v>45017</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -1356,21 +1355,21 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="24">
         <v>45170</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10" s="18"/>
       <c r="I10"/>
@@ -1411,21 +1410,21 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="24">
         <v>45170</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H11" s="18"/>
       <c r="I11"/>
@@ -1466,7 +1465,7 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="24">
         <v>45261</v>
@@ -1474,14 +1473,14 @@
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
       <c r="E12" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I12"/>
       <c r="J12"/>
@@ -1790,16 +1789,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="42"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="34"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1838,23 +1837,23 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H20" s="18"/>
       <c r="I20"/>
@@ -1895,21 +1894,21 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H21" s="18"/>
       <c r="I21"/>
@@ -2174,16 +2173,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="42"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="34"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2222,25 +2221,25 @@
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H28" s="16"/>
       <c r="I28"/>
@@ -2642,6 +2641,11 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2649,11 +2653,6 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>